<commit_message>
added write bisi function
</commit_message>
<xml_diff>
--- a/dbColumns.xlsx
+++ b/dbColumns.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="row format" sheetId="1" r:id="rId1"/>
+    <sheet name="in column format" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>magicPwd</t>
   </si>
@@ -121,13 +121,22 @@
   </si>
   <si>
     <t>personBisiEncashedValue</t>
+  </si>
+  <si>
+    <t>bisiTotalPpl</t>
+  </si>
+  <si>
+    <t>bisiTotalMonths</t>
+  </si>
+  <si>
+    <t>add bisi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +144,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,8 +185,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.26953125" defaultRowHeight="14.5"/>
@@ -581,13 +613,221 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
db test dada added
</commit_message>
<xml_diff>
--- a/dbColumns.xlsx
+++ b/dbColumns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>magicPwd</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>record entry/ partion 4</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>scheme2023</t>
+  </si>
+  <si>
+    <t>emcashed</t>
+  </si>
+  <si>
+    <t>ramesh</t>
   </si>
 </sst>
 </file>
@@ -251,7 +263,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -261,6 +273,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -686,10 +704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C37"/>
+  <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -697,52 +715,65 @@
     <col min="1" max="1" width="29.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.26953125" customWidth="1"/>
     <col min="3" max="3" width="29.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="9">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -752,100 +783,133 @@
       <c r="C10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="10">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="10">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21" s="9">
+        <v>165000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22" s="10">
+        <v>45115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -853,7 +917,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -861,7 +925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
@@ -869,7 +933,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -877,7 +941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
@@ -885,7 +949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
@@ -893,17 +957,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:4">
       <c r="A30" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="D30" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="D31" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>

</xml_diff>